<commit_message>
updated fixed workforce size results output
</commit_message>
<xml_diff>
--- a/rostering_results/results_cm.xlsx
+++ b/rostering_results/results_cm.xlsx
@@ -872,7 +872,7 @@
         <v>20</v>
       </c>
       <c r="J12" t="n">
-        <v>3026.700000000134</v>
+        <v>2981.260000000134</v>
       </c>
     </row>
     <row r="13">
@@ -910,7 +910,7 @@
         <v>20</v>
       </c>
       <c r="J13" t="n">
-        <v>3026.700000000147</v>
+        <v>3026.700000000139</v>
       </c>
     </row>
     <row r="14">
@@ -985,7 +985,9 @@
       <c r="I15" t="n">
         <v>20</v>
       </c>
-      <c r="J15" t="inlineStr"/>
+      <c r="J15" t="n">
+        <v>3606.575000000219</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1093,7 +1095,9 @@
       <c r="I18" t="n">
         <v>20</v>
       </c>
-      <c r="J18" t="inlineStr"/>
+      <c r="J18" t="n">
+        <v>4231.889999999888</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1201,7 +1205,9 @@
       <c r="I21" t="n">
         <v>20</v>
       </c>
-      <c r="J21" t="inlineStr"/>
+      <c r="J21" t="n">
+        <v>4648.766666666827</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1309,7 +1315,9 @@
       <c r="I24" t="n">
         <v>20</v>
       </c>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="n">
+        <v>6357.333333333332</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1767,7 +1775,9 @@
       <c r="I37" t="n">
         <v>20</v>
       </c>
-      <c r="J37" t="inlineStr"/>
+      <c r="J37" t="n">
+        <v>6845.259999999817</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1875,7 +1885,9 @@
       <c r="I40" t="n">
         <v>20</v>
       </c>
-      <c r="J40" t="inlineStr"/>
+      <c r="J40" t="n">
+        <v>8436.574999999741</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1983,7 +1995,9 @@
       <c r="I43" t="n">
         <v>20</v>
       </c>
-      <c r="J43" t="inlineStr"/>
+      <c r="J43" t="n">
+        <v>10027.88999999892</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2091,7 +2105,9 @@
       <c r="I46" t="n">
         <v>20</v>
       </c>
-      <c r="J46" t="inlineStr"/>
+      <c r="J46" t="n">
+        <v>11088.76666666706</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2199,7 +2215,9 @@
       <c r="I49" t="n">
         <v>20</v>
       </c>
-      <c r="J49" t="inlineStr"/>
+      <c r="J49" t="n">
+        <v>13740.95833333339</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2657,7 +2675,9 @@
       <c r="I62" t="n">
         <v>20</v>
       </c>
-      <c r="J62" t="inlineStr"/>
+      <c r="J62" t="n">
+        <v>14565.99333333231</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2765,7 +2785,9 @@
       <c r="I65" t="n">
         <v>20</v>
       </c>
-      <c r="J65" t="inlineStr"/>
+      <c r="J65" t="n">
+        <v>18087.49166666673</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2873,7 +2895,9 @@
       <c r="I68" t="n">
         <v>20</v>
       </c>
-      <c r="J68" t="inlineStr"/>
+      <c r="J68" t="n">
+        <v>21608.98999999871</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2981,7 +3005,9 @@
       <c r="I71" t="n">
         <v>20</v>
       </c>
-      <c r="J71" t="inlineStr"/>
+      <c r="J71" t="n">
+        <v>23956.65555555516</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3089,7 +3115,9 @@
       <c r="I74" t="n">
         <v>20</v>
       </c>
-      <c r="J74" t="inlineStr"/>
+      <c r="J74" t="n">
+        <v>29825.81944444447</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -4761,7 +4789,9 @@
       <c r="I121" t="n">
         <v>20</v>
       </c>
-      <c r="J121" t="inlineStr"/>
+      <c r="J121" t="n">
+        <v>2715.166666666654</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -4869,7 +4899,9 @@
       <c r="I124" t="n">
         <v>20</v>
       </c>
-      <c r="J124" t="inlineStr"/>
+      <c r="J124" t="n">
+        <v>3273.958333333345</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -5327,7 +5359,9 @@
       <c r="I137" t="n">
         <v>20</v>
       </c>
-      <c r="J137" t="inlineStr"/>
+      <c r="J137" t="n">
+        <v>3564.386666666736</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -5435,7 +5469,9 @@
       <c r="I140" t="n">
         <v>20</v>
       </c>
-      <c r="J140" t="inlineStr"/>
+      <c r="J140" t="n">
+        <v>4347.333333333303</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -5543,7 +5579,9 @@
       <c r="I143" t="n">
         <v>20</v>
       </c>
-      <c r="J143" t="inlineStr"/>
+      <c r="J143" t="n">
+        <v>5120.799999999786</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -5651,7 +5689,9 @@
       <c r="I146" t="n">
         <v>20</v>
       </c>
-      <c r="J146" t="inlineStr"/>
+      <c r="J146" t="n">
+        <v>5636.444444444604</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -5759,7 +5799,9 @@
       <c r="I149" t="n">
         <v>20</v>
       </c>
-      <c r="J149" t="inlineStr"/>
+      <c r="J149" t="n">
+        <v>6925.555555555547</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -6217,7 +6259,9 @@
       <c r="I162" t="n">
         <v>20</v>
       </c>
-      <c r="J162" t="inlineStr"/>
+      <c r="J162" t="n">
+        <v>7793.7933333333</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -6325,7 +6369,9 @@
       <c r="I165" t="n">
         <v>20</v>
       </c>
-      <c r="J165" t="inlineStr"/>
+      <c r="J165" t="n">
+        <v>9611.941666666642</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -6433,7 +6479,9 @@
       <c r="I168" t="n">
         <v>20</v>
       </c>
-      <c r="J168" t="inlineStr"/>
+      <c r="J168" t="n">
+        <v>11438.32999999957</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -6541,7 +6589,9 @@
       <c r="I171" t="n">
         <v>20</v>
       </c>
-      <c r="J171" t="inlineStr"/>
+      <c r="J171" t="n">
+        <v>12655.92222222231</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -6649,7 +6699,9 @@
       <c r="I174" t="n">
         <v>20</v>
       </c>
-      <c r="J174" t="inlineStr"/>
+      <c r="J174" t="n">
+        <v>15717.06944444447</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -7997,7 +8049,9 @@
       <c r="I212" t="n">
         <v>20</v>
       </c>
-      <c r="J212" t="inlineStr"/>
+      <c r="J212" t="n">
+        <v>2609.330000000022</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -8105,7 +8159,9 @@
       <c r="I215" t="n">
         <v>20</v>
       </c>
-      <c r="J215" t="inlineStr"/>
+      <c r="J215" t="n">
+        <v>3141.662500000004</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -8213,7 +8269,9 @@
       <c r="I218" t="n">
         <v>20</v>
       </c>
-      <c r="J218" t="inlineStr"/>
+      <c r="J218" t="n">
+        <v>3673.995000000001</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -8321,7 +8379,9 @@
       <c r="I221" t="n">
         <v>20</v>
       </c>
-      <c r="J221" t="inlineStr"/>
+      <c r="J221" t="n">
+        <v>4028.883333333339</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -8429,7 +8489,9 @@
       <c r="I224" t="n">
         <v>20</v>
       </c>
-      <c r="J224" t="inlineStr"/>
+      <c r="J224" t="n">
+        <v>4916.10416666667</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -8887,7 +8949,9 @@
       <c r="I237" t="n">
         <v>20</v>
       </c>
-      <c r="J237" t="inlineStr"/>
+      <c r="J237" t="n">
+        <v>5808.793492063502</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -8995,7 +9059,9 @@
       <c r="I240" t="n">
         <v>20</v>
       </c>
-      <c r="J240" t="inlineStr"/>
+      <c r="J240" t="n">
+        <v>7140.991865079373</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -9103,7 +9169,9 @@
       <c r="I243" t="n">
         <v>20</v>
       </c>
-      <c r="J243" t="inlineStr"/>
+      <c r="J243" t="n">
+        <v>8473.190238095194</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -9211,7 +9279,9 @@
       <c r="I246" t="n">
         <v>20</v>
       </c>
-      <c r="J246" t="inlineStr"/>
+      <c r="J246" t="n">
+        <v>9361.322486772508</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -9319,7 +9389,9 @@
       <c r="I249" t="n">
         <v>20</v>
       </c>
-      <c r="J249" t="inlineStr"/>
+      <c r="J249" t="n">
+        <v>11581.65310846563</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -11557,7 +11629,9 @@
       <c r="I312" t="n">
         <v>20</v>
       </c>
-      <c r="J312" t="inlineStr"/>
+      <c r="J312" t="n">
+        <v>7635.087142857112</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -11665,7 +11739,9 @@
       <c r="I315" t="n">
         <v>20</v>
       </c>
-      <c r="J315" t="inlineStr"/>
+      <c r="J315" t="n">
+        <v>9423.858928571421</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -11773,7 +11849,9 @@
       <c r="I318" t="n">
         <v>20</v>
       </c>
-      <c r="J318" t="inlineStr"/>
+      <c r="J318" t="n">
+        <v>11212.63071428553</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -11881,7 +11959,9 @@
       <c r="I321" t="n">
         <v>20</v>
       </c>
-      <c r="J321" t="inlineStr"/>
+      <c r="J321" t="n">
+        <v>12405.14523809527</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -11989,7 +12069,9 @@
       <c r="I324" t="n">
         <v>20</v>
       </c>
-      <c r="J324" t="inlineStr"/>
+      <c r="J324" t="n">
+        <v>15386.43154761906</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -13337,9 +13419,7 @@
       <c r="I362" t="n">
         <v>20</v>
       </c>
-      <c r="J362" t="n">
-        <v>35848.68849966928</v>
-      </c>
+      <c r="J362" t="inlineStr"/>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -14235,9 +14315,7 @@
       <c r="I387" t="n">
         <v>20</v>
       </c>
-      <c r="J387" t="n">
-        <v>73062.60989546064</v>
-      </c>
+      <c r="J387" t="inlineStr"/>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
@@ -14385,7 +14463,9 @@
       <c r="I391" t="n">
         <v>20</v>
       </c>
-      <c r="J391" t="inlineStr"/>
+      <c r="J391" t="n">
+        <v>91076.38826424249</v>
+      </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
@@ -14421,7 +14501,9 @@
       <c r="I392" t="n">
         <v>20</v>
       </c>
-      <c r="J392" t="inlineStr"/>
+      <c r="J392" t="n">
+        <v>91076.38826424249</v>
+      </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
@@ -14673,9 +14755,7 @@
       <c r="I399" t="n">
         <v>20</v>
       </c>
-      <c r="J399" t="n">
-        <v>151610.4176974274</v>
-      </c>
+      <c r="J399" t="inlineStr"/>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
@@ -14711,9 +14791,7 @@
       <c r="I400" t="n">
         <v>20</v>
       </c>
-      <c r="J400" t="n">
-        <v>151610.4176974274</v>
-      </c>
+      <c r="J400" t="inlineStr"/>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
@@ -14749,9 +14827,7 @@
       <c r="I401" t="n">
         <v>20</v>
       </c>
-      <c r="J401" t="n">
-        <v>151610.4176974274</v>
-      </c>
+      <c r="J401" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>